<commit_message>
Fix image and text output
</commit_message>
<xml_diff>
--- a/output/Times/article6_Times.xlsx
+++ b/output/Times/article6_Times.xlsx
@@ -467,13 +467,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="C2" t="n">
-        <v>399</v>
+        <v>644</v>
       </c>
       <c r="D2" t="n">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="E2" t="n">
         <v>23</v>
@@ -486,13 +486,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C3" t="n">
-        <v>445</v>
+        <v>690</v>
       </c>
       <c r="D3" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E3" t="n">
         <v>23</v>
@@ -505,13 +505,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C4" t="n">
-        <v>1089</v>
+        <v>1334</v>
       </c>
       <c r="D4" t="n">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E4" t="n">
         <v>23</v>
@@ -527,7 +527,7 @@
         <v>446</v>
       </c>
       <c r="C5" t="n">
-        <v>1112</v>
+        <v>1357</v>
       </c>
       <c r="D5" t="n">
         <v>115</v>

</xml_diff>